<commit_message>
add words unit 1-8 to 1-11
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data/words.xlsx
+++ b/backend/src/main/resources/data/words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ysys\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ysys\EnglishWordsTest\backend\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A258514B-4417-47EB-97DD-B003C9EFE51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91266648-2160-43A9-A790-48BAF55FC701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{B611C952-E943-451E-844C-C27BBAE01AA1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="626">
   <si>
     <t>krName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1487,23 +1487,1055 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-7</t>
+    <t>기쁜, 즐거운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화가 난</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>짜증이 난</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>걱정하는, 불안한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우울한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실망한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당황한, 쑥스러운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>긴장한, 초조한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스트레스를 받는</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>속상한, 마음이 상한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만족한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>깜짝 놀란</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건강한, 몸 컨디션이 좋은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건강한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강한, 튼튼한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건강하지 못한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아픈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피로한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몸시 지친, 기진맥진한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>극도로 피곤한, 번아웃된</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠에서 깨다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delighted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>glad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>happy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pleased</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>angry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>furious</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anxious</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>worried</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>annoyed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>irritated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>depressed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disappointed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>embarrassed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nervous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stressed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>satisfied</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>surprised</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>well</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>healthy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>strong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unhealthy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tired</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exhausted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>burnt-out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wake up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일어나다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세수하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>면도하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>샤워하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머리를 감다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머리를 말리다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머리를 빗다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양치질하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치실로 이 사이를 닦다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화장하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>옷을 입다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아침을 먹다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커피를 마시다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차를 마시다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버스를 타다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지하철을 타다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>운전해서 출근하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출근하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wash one's face</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shave</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>take a shower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wash one's hair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dry one's hair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brush one's hair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comb one's hair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brush one's teeth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>floss one's teeth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>put on (one's) makeup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get dressed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eat breakfast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>have breakfast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>have coffee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>have tea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>take the bus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>take the subway</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drive to work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>go to work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점심을 먹다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠깐 쉬다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일을 끝내다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퇴근하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>야근하다, 잔업을 하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저녁을 만들다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저녁을 먹다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TV를 보다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음악을 듣다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>운동하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헬스클럽에서 운동하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인터넷 서핑을 하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소셜미디어를 확인하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sns를 확인하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책을 읽다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잡지를 읽다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목욕하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반신욕을 하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠자리에 들다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>go to bed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>take a half-body bath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>take a lower-body bath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eat lunch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>have lunch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>have a break</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>take a break</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finish work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leave work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get off work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leave the office</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leave for the day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work overtime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cook dinner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make dinner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eat finner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>have dinner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>watch TV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>listen to music</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work out at the gym</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>browse the Internet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>surf the Internet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check social media</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check SNS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read a book</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read a magazine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>take a bath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아침을 만들다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점심을 만들다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도시락을 싸다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>식탁을 차리다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>식탁을 치우다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설거지하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쓰레기를 분리하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쓰레기를 내놓다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집을 청소하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방을 청소하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>욕실을 청소하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방을 치우다, 정리하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책상을 치우다, 정리하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>청소기를 돌리다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빗질을 하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닥을 걸레질하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨래하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨래를 널다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨래를 개다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다리미질을 하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~을 다리다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>침대를 정리하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>침대 시트를 갈다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화초에 물을 주다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반려동물에게 밥을 주다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개에게 밥을 주다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고양이에게 밥을 주다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개를 산책시키다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쇼핑을 하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(식료품) 장을 보다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cook breakfast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make breakfast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cook lunch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make lunch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make a lunchbox</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set the table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear the table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wash the dishes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>do the dishes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>take out the trash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clean the house</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>separate trash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clean the room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clean the bathroom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clean up one's room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clean up one's desk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vacuum the floor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sweep the floor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mop the floor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>do the laundry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wash the clothes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hang the clothes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flod the clothes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>do the ironing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron ~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make the bed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>change the sheets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>water the plants</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feed the pet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feed the dog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feed the cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>walk the dog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>do the shopping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>do grocery shopping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새해 첫날</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설날</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼일절</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>식목일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어린이날</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어버이날</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>석가탄신일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현충일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제헌절</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>광복절</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개천절</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한글날</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크리스마스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12월 31일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첫돌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환갑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>칠순</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결혼기념일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집들이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>송별회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환영회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>송년회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Year's Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lunar New Year's Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Korean New Year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Independence Movement Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arbor Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Children's Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parent's Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buddha's Birthday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memorial Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Constitution Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liberation Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chuseok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Korean Thanksgiving Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>National Foundation Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hangul Proclamation Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Christmas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Christmas Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Year's Eve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100th day after birth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the first birthday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the sixtieth birthday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the seventieth birthday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wedding anniversary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>housewarming party</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>farewell party</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>welcome party</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>year-end party</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anniversary of one's death</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>104</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>105</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>106</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>107</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>108</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>109</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1874,16 +2906,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D114FCA-6A6B-4805-9CCE-50B88DAEF0B4}">
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C342"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="40.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.6640625" style="1"/>
   </cols>
@@ -1907,7 +2939,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -1918,7 +2950,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -1929,7 +2961,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -1940,7 +2972,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -1951,7 +2983,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -1962,7 +2994,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -1973,7 +3005,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -1984,7 +3016,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -1995,7 +3027,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -2006,7 +3038,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -2017,7 +3049,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -2028,7 +3060,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -2039,7 +3071,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -2050,7 +3082,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -2061,7 +3093,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -2072,7 +3104,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -2083,7 +3115,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -2094,7 +3126,7 @@
         <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -2105,7 +3137,7 @@
         <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -2116,7 +3148,7 @@
         <v>42</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -2127,7 +3159,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -2138,7 +3170,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -2149,7 +3181,7 @@
         <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -2160,7 +3192,7 @@
         <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -2171,7 +3203,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -2182,7 +3214,7 @@
         <v>51</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -2193,7 +3225,7 @@
         <v>60</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -2204,7 +3236,7 @@
         <v>61</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -2215,7 +3247,7 @@
         <v>62</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -2226,7 +3258,7 @@
         <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
@@ -2237,7 +3269,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -2248,7 +3280,7 @@
         <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
@@ -2259,7 +3291,7 @@
         <v>66</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -2270,7 +3302,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>363</v>
+        <v>617</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
@@ -2281,7 +3313,7 @@
         <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -2292,7 +3324,7 @@
         <v>71</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
@@ -2303,7 +3335,7 @@
         <v>72</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
@@ -2314,7 +3346,7 @@
         <v>73</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -2325,7 +3357,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -2336,7 +3368,7 @@
         <v>75</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
@@ -2347,7 +3379,7 @@
         <v>76</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -2358,7 +3390,7 @@
         <v>77</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -2369,7 +3401,7 @@
         <v>78</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
@@ -2380,7 +3412,7 @@
         <v>73</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -2391,7 +3423,7 @@
         <v>74</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
@@ -2402,7 +3434,7 @@
         <v>81</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -2413,7 +3445,7 @@
         <v>82</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
@@ -2424,7 +3456,7 @@
         <v>83</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
@@ -2435,7 +3467,7 @@
         <v>84</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
@@ -2446,7 +3478,7 @@
         <v>81</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
@@ -2457,7 +3489,7 @@
         <v>85</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
@@ -2468,7 +3500,7 @@
         <v>86</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
@@ -2479,7 +3511,7 @@
         <v>87</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>364</v>
+        <v>618</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
@@ -2490,7 +3522,7 @@
         <v>113</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
@@ -2501,7 +3533,7 @@
         <v>114</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
@@ -2512,7 +3544,7 @@
         <v>115</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
@@ -2523,7 +3555,7 @@
         <v>116</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
@@ -2534,7 +3566,7 @@
         <v>117</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
@@ -2545,7 +3577,7 @@
         <v>118</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
@@ -2556,7 +3588,7 @@
         <v>119</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
@@ -2567,7 +3599,7 @@
         <v>120</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
@@ -2578,7 +3610,7 @@
         <v>121</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
@@ -2589,7 +3621,7 @@
         <v>122</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
@@ -2600,7 +3632,7 @@
         <v>123</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
@@ -2611,7 +3643,7 @@
         <v>124</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
@@ -2622,7 +3654,7 @@
         <v>125</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
@@ -2633,7 +3665,7 @@
         <v>104</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
@@ -2644,7 +3676,7 @@
         <v>105</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
@@ -2655,7 +3687,7 @@
         <v>106</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
@@ -2666,7 +3698,7 @@
         <v>107</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
@@ -2677,7 +3709,7 @@
         <v>126</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
@@ -2688,7 +3720,7 @@
         <v>127</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
@@ -2699,7 +3731,7 @@
         <v>128</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
@@ -2710,7 +3742,7 @@
         <v>129</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
@@ -2721,7 +3753,7 @@
         <v>130</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
@@ -2732,7 +3764,7 @@
         <v>149</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
@@ -2743,7 +3775,7 @@
         <v>150</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
@@ -2754,7 +3786,7 @@
         <v>151</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
@@ -2765,7 +3797,7 @@
         <v>152</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
@@ -2776,7 +3808,7 @@
         <v>153</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
@@ -2787,7 +3819,7 @@
         <v>154</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
@@ -2798,7 +3830,7 @@
         <v>155</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
@@ -2809,7 +3841,7 @@
         <v>156</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
@@ -2820,7 +3852,7 @@
         <v>157</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
@@ -2831,7 +3863,7 @@
         <v>158</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
@@ -2842,7 +3874,7 @@
         <v>159</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
@@ -2853,7 +3885,7 @@
         <v>160</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
@@ -2864,7 +3896,7 @@
         <v>161</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
@@ -2875,7 +3907,7 @@
         <v>162</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
@@ -2886,7 +3918,7 @@
         <v>163</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
@@ -2897,7 +3929,7 @@
         <v>164</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
@@ -2908,7 +3940,7 @@
         <v>165</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
@@ -2919,7 +3951,7 @@
         <v>166</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>365</v>
+        <v>619</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
@@ -2930,7 +3962,7 @@
         <v>185</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
@@ -2941,7 +3973,7 @@
         <v>186</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
@@ -2952,7 +3984,7 @@
         <v>86</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
@@ -2963,7 +3995,7 @@
         <v>187</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
@@ -2974,7 +4006,7 @@
         <v>188</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
@@ -2985,7 +4017,7 @@
         <v>189</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
@@ -2996,7 +4028,7 @@
         <v>190</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
@@ -3007,7 +4039,7 @@
         <v>191</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
@@ -3018,7 +4050,7 @@
         <v>192</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
@@ -3029,7 +4061,7 @@
         <v>193</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
@@ -3040,7 +4072,7 @@
         <v>194</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
@@ -3051,7 +4083,7 @@
         <v>195</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
@@ -3062,7 +4094,7 @@
         <v>196</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
@@ -3073,7 +4105,7 @@
         <v>197</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
@@ -3084,7 +4116,7 @@
         <v>198</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
@@ -3095,7 +4127,7 @@
         <v>199</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
@@ -3106,7 +4138,7 @@
         <v>200</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
@@ -3117,7 +4149,7 @@
         <v>201</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
@@ -3128,7 +4160,7 @@
         <v>202</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
@@ -3139,7 +4171,7 @@
         <v>203</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
@@ -3150,7 +4182,7 @@
         <v>224</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
@@ -3161,7 +4193,7 @@
         <v>225</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
@@ -3172,7 +4204,7 @@
         <v>226</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
@@ -3183,7 +4215,7 @@
         <v>227</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
@@ -3194,7 +4226,7 @@
         <v>116</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
@@ -3205,7 +4237,7 @@
         <v>123</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
@@ -3216,7 +4248,7 @@
         <v>228</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
@@ -3227,7 +4259,7 @@
         <v>229</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
@@ -3238,7 +4270,7 @@
         <v>230</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
@@ -3249,7 +4281,7 @@
         <v>231</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
@@ -3260,7 +4292,7 @@
         <v>232</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
@@ -3271,7 +4303,7 @@
         <v>233</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
@@ -3282,7 +4314,7 @@
         <v>234</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
@@ -3293,7 +4325,7 @@
         <v>235</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
@@ -3304,7 +4336,7 @@
         <v>236</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
@@ -3315,7 +4347,7 @@
         <v>237</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
@@ -3326,7 +4358,7 @@
         <v>238</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
@@ -3337,7 +4369,7 @@
         <v>239</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
@@ -3348,7 +4380,7 @@
         <v>240</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
@@ -3359,7 +4391,7 @@
         <v>241</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
@@ -3370,7 +4402,7 @@
         <v>242</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
@@ -3381,7 +4413,7 @@
         <v>272</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
@@ -3392,7 +4424,7 @@
         <v>273</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
@@ -3403,7 +4435,7 @@
         <v>274</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
@@ -3414,7 +4446,7 @@
         <v>275</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
@@ -3425,7 +4457,7 @@
         <v>276</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
@@ -3436,7 +4468,7 @@
         <v>277</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
@@ -3447,7 +4479,7 @@
         <v>278</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
@@ -3458,7 +4490,7 @@
         <v>279</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
@@ -3469,7 +4501,7 @@
         <v>280</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
@@ -3480,7 +4512,7 @@
         <v>281</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
@@ -3491,7 +4523,7 @@
         <v>282</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
@@ -3502,7 +4534,7 @@
         <v>283</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
@@ -3513,7 +4545,7 @@
         <v>284</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
@@ -3524,7 +4556,7 @@
         <v>285</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
@@ -3535,7 +4567,7 @@
         <v>286</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
@@ -3546,7 +4578,7 @@
         <v>287</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
@@ -3557,7 +4589,7 @@
         <v>288</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
@@ -3568,7 +4600,7 @@
         <v>289</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
@@ -3579,7 +4611,7 @@
         <v>290</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
@@ -3590,7 +4622,7 @@
         <v>291</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
@@ -3601,7 +4633,7 @@
         <v>292</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
@@ -3612,7 +4644,7 @@
         <v>293</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
@@ -3623,7 +4655,7 @@
         <v>294</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
@@ -3634,7 +4666,7 @@
         <v>295</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
@@ -3645,7 +4677,7 @@
         <v>296</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
@@ -3656,7 +4688,7 @@
         <v>297</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
@@ -3667,7 +4699,7 @@
         <v>298</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
@@ -3678,7 +4710,7 @@
         <v>299</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
@@ -3689,7 +4721,7 @@
         <v>300</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>366</v>
+        <v>620</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.45">
@@ -3700,7 +4732,7 @@
         <v>329</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.45">
@@ -3711,7 +4743,7 @@
         <v>330</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
@@ -3722,7 +4754,7 @@
         <v>331</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.45">
@@ -3733,7 +4765,7 @@
         <v>332</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.45">
@@ -3744,7 +4776,7 @@
         <v>333</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.45">
@@ -3755,7 +4787,7 @@
         <v>334</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.45">
@@ -3766,7 +4798,7 @@
         <v>335</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.45">
@@ -3777,7 +4809,7 @@
         <v>336</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.45">
@@ -3788,7 +4820,7 @@
         <v>337</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.45">
@@ -3799,7 +4831,7 @@
         <v>338</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.45">
@@ -3810,7 +4842,7 @@
         <v>339</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.45">
@@ -3821,7 +4853,7 @@
         <v>340</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.45">
@@ -3832,7 +4864,7 @@
         <v>341</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.45">
@@ -3843,7 +4875,7 @@
         <v>342</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.45">
@@ -3854,7 +4886,7 @@
         <v>343</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.45">
@@ -3865,7 +4897,7 @@
         <v>344</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.45">
@@ -3876,7 +4908,7 @@
         <v>345</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.45">
@@ -3887,7 +4919,7 @@
         <v>346</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.45">
@@ -3898,7 +4930,7 @@
         <v>347</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.45">
@@ -3909,7 +4941,7 @@
         <v>348</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.45">
@@ -3920,7 +4952,7 @@
         <v>349</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.45">
@@ -3931,7 +4963,7 @@
         <v>350</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.45">
@@ -3942,7 +4974,7 @@
         <v>351</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.45">
@@ -3953,7 +4985,7 @@
         <v>352</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.45">
@@ -3964,7 +4996,7 @@
         <v>353</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.45">
@@ -3975,7 +5007,7 @@
         <v>354</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.45">
@@ -3986,7 +5018,7 @@
         <v>355</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.45">
@@ -3997,7 +5029,7 @@
         <v>356</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.45">
@@ -4008,7 +5040,7 @@
         <v>357</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.45">
@@ -4019,7 +5051,7 @@
         <v>358</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.45">
@@ -4030,7 +5062,7 @@
         <v>359</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.45">
@@ -4041,7 +5073,7 @@
         <v>360</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.45">
@@ -4052,7 +5084,7 @@
         <v>361</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>367</v>
+        <v>621</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.45">
@@ -4063,7 +5095,1591 @@
         <v>362</v>
       </c>
       <c r="C198" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A199" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A200" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A201" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A202" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A203" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A204" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A205" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A206" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A207" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A208" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A209" s="1" t="s">
         <v>367</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A210" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A211" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A212" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A213" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A214" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A215" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A216" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A217" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A218" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A219" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A220" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A221" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A222" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A223" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A224" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A225" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A226" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A227" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A228" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A229" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A230" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A231" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A232" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A233" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A234" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A235" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A236" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A237" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A238" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A239" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A240" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A241" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A242" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A243" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A244" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A245" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A246" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A247" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A248" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A249" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A250" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A251" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A252" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A253" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A254" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A255" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A256" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A257" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A258" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A259" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A260" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A261" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A262" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A263" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A264" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A265" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A266" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A267" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A268" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A269" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A270" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A271" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A272" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A273" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A274" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A275" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A276" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A277" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A278" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A279" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A280" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A281" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A282" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A283" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A284" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A285" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A286" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A287" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A288" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A289" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A290" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A291" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A292" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A293" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A294" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A295" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A296" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A297" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A298" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A299" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A300" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A301" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A302" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A303" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A304" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A305" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A306" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A307" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A308" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A309" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A310" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A311" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A312" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A313" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A314" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A315" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A316" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A317" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A318" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A319" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A320" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A321" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A322" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A323" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A324" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A325" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A326" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A327" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A328" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A329" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A330" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A331" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A332" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C332" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A333" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="C333" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A334" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="C334" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A335" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A336" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="C336" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A337" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="C337" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A338" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="C338" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A339" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C339" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A340" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="C340" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A341" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="C341" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A342" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add words in excel
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data/words.xlsx
+++ b/backend/src/main/resources/data/words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ysys\EnglishWordsTest\backend\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91266648-2160-43A9-A790-48BAF55FC701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8459275-A141-4612-AA21-47FFADE95393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{B611C952-E943-451E-844C-C27BBAE01AA1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="954">
   <si>
     <t>krName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2536,6 +2536,1313 @@
   </si>
   <si>
     <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어깨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머리카락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>얼굴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>흉부, 가슴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>젖꼭지, 유두</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배, 복부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배꼽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무릎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정강이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발가락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발톱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팔꿈치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손가락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손톱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엉덩이, 히프, 둔부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엉덩이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허벅지, 넓적다리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종아리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유방, (여성의) 가슴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등, (등) 허리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upper body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lower body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>head</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>face</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>neck</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shoulder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nipple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stomach</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>navel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>belly button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>knee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>toe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>toenail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>back</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>elbow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wrist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fingernail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pelvis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buttocks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>butt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thigh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ankle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>breast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bust</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>202</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>귀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>광대뼈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>볼, 뺨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입술</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>턱 (아래턱, 턱 끝)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>턱 (턱뼈 전체)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관자놀이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콧구멍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>눈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>눈썹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>속눈썹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>눈꺼풀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외까풀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쌍꺼풀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>눈동자, 동공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이, 치아 (단수)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이, 치아 (복수)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잇몸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윗니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아랫니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앞니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>송곳니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어금니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>덧니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사랑니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집게손가락, 검지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엄지손가락, 엄지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가운뎃손가락, 중지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>넷째손가락, 약지, 무명지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새끼손가락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손바닥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주먹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엄지발가락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>둘째발가락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>셋째발가락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>넷째발가락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새끼발가락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발바닥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발뒤꿈치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forehead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cheekbone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cheek</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jaw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nose</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nostril</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mouth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eye</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eyebrow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eyelashes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eyelid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>single eyelid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double eyelid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pupil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tooth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teeth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upper tooth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lower tooth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>front tooth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>canine tooth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>molar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tongue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snaggle tooth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wisdom tooth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index finger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thumb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>back of one's hand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>middle finger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ring finger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>little finger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>palm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>big toe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>top of the foot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>second toe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>third toe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fourth toe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>little toe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sole</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>203</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>살</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피, 혈액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뇌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뼈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근육</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>힘줄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동맥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정맥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혈관</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신경세포, 뉴런</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세포</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목 (구멍)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>갑상선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>폐, 허파</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쓸개, 담낭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장, 창자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>심장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>췌장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콩팥, 신장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방광</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>두개골</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목뼈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>척추</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골반뼈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관절</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뼈대, 골격, 해골</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쇄골</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>갈비뼈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>흉골</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flesh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nerve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>muscle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tendon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>artery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vein</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blood vessel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>veuron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>throat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thyroid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gallbladder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>large intestine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>small intestine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bowel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pancreas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kidney</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bladder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skull</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>neck bone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>backbone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pelvic bone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>joint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skeleton</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collarbone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rib</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>breast bone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>눈물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>땀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>침</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가래</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>눈곱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>귀지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소변</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대변</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sweat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>saliva</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phlegm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sleep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>earwax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>urine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>excrement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키가 작은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>204</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중간 키(의)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평균 키(의)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키가 큰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날씬한, 호리호리한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비쩍 마른</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통통한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과체중의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비만인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뚱뚱한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근육질의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중년의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>늙은, 나이 많은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연세가 드신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘생긴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(주로 남자가) 잘생긴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멋진, 매력적인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매력적인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(주로 여성이나 아이가) 아름다운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예쁜, 귀여운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사랑스러운, 매력적인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>살이 찌다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>살이 빠지다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다이어트 중이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50대</t>
+  </si>
+  <si>
+    <t>60대</t>
+  </si>
+  <si>
+    <t>70대</t>
+  </si>
+  <si>
+    <t>80대</t>
+  </si>
+  <si>
+    <t>90대</t>
+  </si>
+  <si>
+    <t>초반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>후반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~ 또래다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>medium height</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>average height</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slender</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skinny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chubby</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overweight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>obese</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>muscular</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>middle-aged</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>old</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>elderly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>good-looking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>handsome</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gorgeous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attractive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beautiful</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pretty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lovely</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gain weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lose weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>be on a diet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teens</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>twenties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thirties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fifties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sixties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seventies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eighties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nineties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>one's early ~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>one's mid ~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>one's late ~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>about one's age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>around one's age</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2906,10 +4213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D114FCA-6A6B-4805-9CCE-50B88DAEF0B4}">
-  <dimension ref="A1:C342"/>
+  <dimension ref="A1:C513"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A496" workbookViewId="0">
+      <selection activeCell="D514" sqref="D514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -6682,6 +7989,1887 @@
         <v>625</v>
       </c>
     </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A343" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="C343" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A344" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A345" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="C345" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A346" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="C346" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A347" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="C347" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A348" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="C348" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A349" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C349" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A350" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="C350" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A351" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A352" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A353" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="C353" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A354" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="C354" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A355" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="C355" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A356" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A357" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A358" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A359" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A360" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A361" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A362" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="C362" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A363" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="C363" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A364" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="C364" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A365" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="C365" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A366" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="C366" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A367" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A368" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A369" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A370" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A371" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A372" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A373" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A374" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A375" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A376" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A377" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A378" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C378" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A379" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A380" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="C380" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A381" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="C381" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A382" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A383" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A384" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="C384" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A385" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="C385" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A386" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="C386" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A387" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="C387" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A388" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C388" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A389" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="C389" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A390" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A391" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A392" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C392" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A393" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="C393" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A394" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="C394" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A395" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="C395" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A396" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="C396" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A397" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A398" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C398" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A399" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="C399" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A400" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C400" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A401" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="C401" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A402" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="C402" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A403" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A404" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="C404" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A405" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="C405" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A406" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="C406" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A407" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="C407" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A408" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="C408" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A409" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="C409" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A410" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="C410" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A411" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="C411" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A412" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="C412" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A413" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="C413" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A414" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="C414" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A415" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="C415" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A416" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="C416" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A417" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="C417" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A418" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="C418" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A419" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="C419" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A420" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="C420" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A421" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="C421" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A422" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C422" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A423" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="C423" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A424" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="C424" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A425" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="C425" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A426" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="C426" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A427" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C427" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A428" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="C428" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A429" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="C429" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A430" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="C430" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A431" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="C431" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A432" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="C432" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A433" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="C433" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A434" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B434" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="C434" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A435" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="C435" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A436" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C436" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A437" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="C437" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A438" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C438" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A439" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B439" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C439" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A440" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B440" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="C440" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A441" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="C441" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A442" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="B442" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="C442" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A443" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B443" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="C443" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A444" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C444" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A445" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B445" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="C445" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A446" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B446" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="C446" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A447" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="C447" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A448" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="C448" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A449" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="C449" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A450" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="C450" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A451" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="C451" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A452" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="C452" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A453" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="C453" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A454" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="C454" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A455" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="C455" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A456" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="C456" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A457" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="C457" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A458" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C458" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A459" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="C459" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A460" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C460" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A461" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C461" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A462" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="C462" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A463" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C463" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A464" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="C464" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A465" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="B465" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="C465" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A466" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="C466" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A467" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="C467" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A468" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="B468" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="C468" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A469" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B469" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="C469" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A470" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="C470" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A471" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="B471" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="C471" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A472" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="B472" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C472" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A473" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="B473" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="C473" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A474" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B474" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="C474" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A475" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C475" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A476" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B476" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="C476" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A477" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="C477" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A478" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="C478" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A479" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C479" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A480" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B480" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="C480" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A481" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B481" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="C481" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A482" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B482" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="C482" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A483" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="C483" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A484" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="C484" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A485" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="C485" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A486" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="C486" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A487" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B487" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C487" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A488" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="C488" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A489" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="B489" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="C489" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A490" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="C490" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A491" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="C491" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A492" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="C492" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A493" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C493" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A494" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="C494" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A495" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="C495" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A496" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="C496" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A497" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="C497" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A498" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="C498" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A499" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="C499" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A500" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="C500" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A501" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="C501" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A502" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="C502" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A503" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="C503" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A504" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="C504" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A505" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="C505" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A506" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="C506" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A507" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="C507" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A508" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="C508" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A509" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="C509" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A510" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="C510" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A511" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C511" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A512" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="C512" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A513" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="C513" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>